<commit_message>
Gabriel de Moura Silva - grafico de burndown
</commit_message>
<xml_diff>
--- a/Documentação/burndown.xlsx
+++ b/Documentação/burndown.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmsil\Documents\LibugGC222\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E74A5EC-5B76-46CD-96BA-892E837B932B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0AF05446-85C1-4570-8426-0394781725C3}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="5145" xr2:uid="{163BE9DC-8C92-4CC2-88F8-CB5591166C0F}"/>
   </bookViews>
@@ -430,13 +430,13 @@
                   <c:v>335</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>#N/A</c:v>
+                  <c:v>330</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>#N/A</c:v>
+                  <c:v>325</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>#N/A</c:v>
+                  <c:v>223</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>#N/A</c:v>
@@ -1730,8 +1730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FAECB3D-C896-4300-9121-B22DE38897E9}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AM9" sqref="AM9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1812,8 +1812,12 @@
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>5</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -1888,9 +1892,13 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1">
+        <v>42</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -1924,9 +1932,13 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1">
+        <v>18</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1960,9 +1972,13 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="G11" s="1">
+        <v>20</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1978,9 +1994,13 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="G12" s="1">
+        <v>22</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -2137,17 +2157,17 @@
         <f t="shared" ref="D20:L20" si="0">IF(SUM(D2:D19)&gt;0,C20-SUM(D2:D19),NA())</f>
         <v>335</v>
       </c>
-      <c r="E20" s="3" t="e">
+      <c r="E20" s="3">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F20" s="3" t="e">
+        <v>330</v>
+      </c>
+      <c r="F20" s="3">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="G20" s="3" t="e">
+        <v>325</v>
+      </c>
+      <c r="G20" s="3">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>223</v>
       </c>
       <c r="H20" s="3" t="e">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Atualizacao do Burndown 15-06
</commit_message>
<xml_diff>
--- a/Documentação/burndown.xlsx
+++ b/Documentação/burndown.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmsil\Documents\LibugGC222\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\OneDrive\Documentos\UniRV\7º Periodo\Gerencia de Configuração\03 - Biblioteca\LibBugGC\LibBugGC\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0AF05446-85C1-4570-8426-0394781725C3}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{64305A76-64F8-4E39-9F7C-114D9094366F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="5145" xr2:uid="{163BE9DC-8C92-4CC2-88F8-CB5591166C0F}"/>
   </bookViews>
@@ -439,7 +439,7 @@
                   <c:v>223</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>#N/A</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>#N/A</c:v>
@@ -1731,7 +1731,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1819,7 +1819,9 @@
         <v>5</v>
       </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="H3" s="1">
+        <v>3</v>
+      </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -1899,7 +1901,9 @@
       <c r="G7" s="1">
         <v>42</v>
       </c>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1">
+        <v>40</v>
+      </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -1939,7 +1943,9 @@
       <c r="G9" s="1">
         <v>18</v>
       </c>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1">
+        <v>19</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1979,7 +1985,9 @@
       <c r="G11" s="1">
         <v>20</v>
       </c>
-      <c r="H11" s="1"/>
+      <c r="H11" s="1">
+        <v>21</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -2001,7 +2009,9 @@
       <c r="G12" s="1">
         <v>22</v>
       </c>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1">
+        <v>22</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -2169,9 +2179,9 @@
         <f t="shared" si="0"/>
         <v>223</v>
       </c>
-      <c r="H20" s="3" t="e">
+      <c r="H20" s="3">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>118</v>
       </c>
       <c r="I20" s="3" t="e">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Atualizacao do BurnDown 21/06
</commit_message>
<xml_diff>
--- a/Documentação/burndown.xlsx
+++ b/Documentação/burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\OneDrive\Documentos\UniRV\7º Periodo\Gerencia de Configuração\03 - Biblioteca\LibBugGC\LibBugGC\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{13467FB3-8080-41C6-95B3-D06892631B1E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8D8877BF-E111-4792-9215-5224689B9195}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="5145" xr2:uid="{163BE9DC-8C92-4CC2-88F8-CB5591166C0F}"/>
   </bookViews>
@@ -175,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -183,6 +183,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,9 +376,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Planilha1!$B$1:$L$1</c:f>
+              <c:f>Planilha1!$B$1:$I$1</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Peso</c:v>
                 </c:pt>
@@ -401,25 +402,16 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>21/06/2018</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>28/06/2018</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>05/07/2018</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12/07/2018</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$B$20:$L$20</c:f>
+              <c:f>Planilha1!$B$20:$I$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>496</c:v>
                 </c:pt>
@@ -439,19 +431,10 @@
                   <c:v>223</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>118</c:v>
+                  <c:v>158</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -551,9 +534,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Planilha1!$B$1:$L$1</c:f>
+              <c:f>Planilha1!$B$1:$I$1</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Peso</c:v>
                 </c:pt>
@@ -577,57 +560,39 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>21/06/2018</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>28/06/2018</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>05/07/2018</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12/07/2018</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$B$21:$L$21</c:f>
+              <c:f>Planilha1!$B$21:$I$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>496</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>446.4</c:v>
+                  <c:v>425.14285714285711</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>396.79999999999995</c:v>
+                  <c:v>354.28571428571422</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>347.19999999999993</c:v>
+                  <c:v>283.42857142857133</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>297.59999999999991</c:v>
+                  <c:v>212.57142857142847</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>247.99999999999991</c:v>
+                  <c:v>141.71428571428561</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>198.39999999999992</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>148.79999999999993</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>99.199999999999932</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>49.59999999999993</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>70.857142857142748</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="m/d/yyyy">
+                  <c:v>-1.1368683772161603E-13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1394,16 +1359,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>117101</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>280386</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>56028</xdr:rowOff>
+      <xdr:rowOff>110457</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>449036</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:rowOff>173491</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1728,10 +1693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FAECB3D-C896-4300-9121-B22DE38897E9}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AL43" sqref="AL43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1741,11 +1706,9 @@
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1771,17 +1734,8 @@
       <c r="I1" s="6">
         <v>43272</v>
       </c>
-      <c r="J1" s="6">
-        <v>43279</v>
-      </c>
-      <c r="K1" s="6">
-        <v>43286</v>
-      </c>
-      <c r="L1" s="6">
-        <v>43293</v>
-      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1798,12 +1752,15 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="I2" s="1">
+        <v>7</v>
+      </c>
+      <c r="J2">
+        <f>B2-SUM(C2:I2)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1825,11 +1782,12 @@
         <v>3</v>
       </c>
       <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
+      <c r="J3">
+        <f>B3-SUM(C3:I3)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1842,12 +1800,15 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
+      <c r="I4" s="1">
+        <v>15</v>
+      </c>
+      <c r="J4">
+        <f>B4-SUM(C4:I4)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1860,12 +1821,15 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
+      <c r="I5" s="1">
+        <v>30</v>
+      </c>
+      <c r="J5">
+        <f>B5-SUM(C5:I5)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1883,11 +1847,12 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
+      <c r="J6">
+        <f>B6-SUM(C6:I6)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1907,11 +1872,12 @@
         <v>40</v>
       </c>
       <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+      <c r="J7">
+        <f>B7-SUM(C7:I7)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -1924,12 +1890,15 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
+      <c r="I8" s="1">
+        <v>30</v>
+      </c>
+      <c r="J8">
+        <f>B8-SUM(C8:I8)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -1949,11 +1918,12 @@
         <v>19</v>
       </c>
       <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
+      <c r="J9">
+        <f>B9-SUM(C9:I9)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -1966,12 +1936,15 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
+      <c r="I10" s="1">
+        <v>13</v>
+      </c>
+      <c r="J10">
+        <f>B10-SUM(C10:I10)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1988,14 +1961,15 @@
         <v>20</v>
       </c>
       <c r="H11" s="1">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
+      <c r="J11">
+        <f>B11-SUM(C11:I11)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
@@ -2012,14 +1986,15 @@
         <v>22</v>
       </c>
       <c r="H12" s="1">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
+      <c r="J12">
+        <f>B12-SUM(C12:I12)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -2032,12 +2007,15 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
+      <c r="I13" s="1">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <f>B13-SUM(C13:I13)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -2055,11 +2033,12 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
+      <c r="J14">
+        <f>B14-SUM(C14:I14)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
@@ -2077,11 +2056,12 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
+      <c r="J15">
+        <f>B15-SUM(C15:I15)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
@@ -2094,12 +2074,15 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
+      <c r="I16" s="1">
+        <v>23</v>
+      </c>
+      <c r="J16">
+        <f>B16-SUM(C16:I16)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
@@ -2112,12 +2095,15 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
+      <c r="I17" s="1">
+        <v>15</v>
+      </c>
+      <c r="J17">
+        <f>B17-SUM(C17:I17)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
@@ -2130,12 +2116,15 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
+      <c r="I18" s="1">
+        <v>23</v>
+      </c>
+      <c r="J18">
+        <f>B18-SUM(C18:I18)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
@@ -2149,11 +2138,12 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
+      <c r="J19">
+        <f>B19-SUM(C19:I19)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>1</v>
       </c>
@@ -2166,7 +2156,7 @@
         <v>492</v>
       </c>
       <c r="D20" s="3">
-        <f t="shared" ref="D20:L20" si="0">IF(SUM(D2:D19)&gt;0,C20-SUM(D2:D19),NA())</f>
+        <f t="shared" ref="D20:I20" si="0">IF(SUM(D2:D19)&gt;0,C20-SUM(D2:D19),NA())</f>
         <v>335</v>
       </c>
       <c r="E20" s="3">
@@ -2183,26 +2173,14 @@
       </c>
       <c r="H20" s="3">
         <f t="shared" si="0"/>
-        <v>118</v>
-      </c>
-      <c r="I20" s="3" t="e">
+        <v>158</v>
+      </c>
+      <c r="I20" s="3">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J20" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="K20" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="L20" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>2</v>
       </c>
@@ -2211,43 +2189,32 @@
         <v>496</v>
       </c>
       <c r="C21" s="3">
-        <f>B21-($B$21/COUNTA($C$1:$L$1))</f>
-        <v>446.4</v>
+        <f>B21-($B$21/COUNTA($C$1:$I$1))</f>
+        <v>425.14285714285711</v>
       </c>
       <c r="D21" s="3">
-        <f t="shared" ref="D21:K21" si="1">C21-($B$21/COUNTA($C$1:$L$1))</f>
-        <v>396.79999999999995</v>
+        <f>C21-($B$21/COUNTA($C$1:$I$1))</f>
+        <v>354.28571428571422</v>
       </c>
       <c r="E21" s="3">
-        <f t="shared" si="1"/>
-        <v>347.19999999999993</v>
+        <f>D21-($B$21/COUNTA($C$1:$I$1))</f>
+        <v>283.42857142857133</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" si="1"/>
-        <v>297.59999999999991</v>
+        <f>E21-($B$21/COUNTA($C$1:$I$1))</f>
+        <v>212.57142857142847</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" si="1"/>
-        <v>247.99999999999991</v>
+        <f>F21-($B$21/COUNTA($C$1:$I$1))</f>
+        <v>141.71428571428561</v>
       </c>
       <c r="H21" s="3">
-        <f t="shared" si="1"/>
-        <v>198.39999999999992</v>
-      </c>
-      <c r="I21" s="3">
-        <f t="shared" si="1"/>
-        <v>148.79999999999993</v>
-      </c>
-      <c r="J21" s="3">
-        <f>I21-($B$21/COUNTA($C$1:$L$1))</f>
-        <v>99.199999999999932</v>
-      </c>
-      <c r="K21" s="3">
-        <f t="shared" si="1"/>
-        <v>49.59999999999993</v>
-      </c>
-      <c r="L21" s="3">
-        <v>0</v>
+        <f>G21-($B$21/COUNTA($C$1:$I$1))</f>
+        <v>70.857142857142748</v>
+      </c>
+      <c r="I21" s="7">
+        <f>H21-($B$21/COUNTA($C$1:$I$1))</f>
+        <v>-1.1368683772161603E-13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>